<commit_message>
fix: [#64663] Fix template
</commit_message>
<xml_diff>
--- a/akap/udbytte/static/xlsx/skabelon.xlsx
+++ b/akap/udbytte/static/xlsx/skabelon.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">Generalforsamlingsdato</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Udbetalingsdato</t>
   </si>
@@ -61,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -82,6 +80,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,13 +151,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -190,9 +189,6 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>